<commit_message>
add PDF print of schematic
</commit_message>
<xml_diff>
--- a/bom/bath_clamp_bom.xlsx
+++ b/bom/bath_clamp_bom.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/My Drive/UST/research/covg/pcb_design/kicad/covg_clamp/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCE5D650-EF9F-434F-BBE4-AE4F9393D823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36820C51-3FDC-4945-B52D-A0F3B6BA0A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440"/>
+    <workbookView minimized="1" xWindow="43220" yWindow="-300" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bath_clamp" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1225,7 +1237,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2060,15 +2072,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M261"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
+      <selection activeCell="I251" sqref="I251"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="7" max="7" width="31.33203125" customWidth="1"/>
-    <col min="8" max="8" width="27.33203125" customWidth="1"/>
+    <col min="8" max="8" width="27.33203125" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>